<commit_message>
- report ready for proofreading
</commit_message>
<xml_diff>
--- a/MovingAveragesExamples.xlsx
+++ b/MovingAveragesExamples.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="SMA" sheetId="1" r:id="rId1"/>
     <sheet name="CMA" sheetId="2" r:id="rId2"/>
     <sheet name="WMA" sheetId="3" r:id="rId3"/>
     <sheet name="EWMA" sheetId="4" r:id="rId4"/>
+    <sheet name="Peak Detection Example" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="15">
   <si>
     <t>Observation Value</t>
   </si>
@@ -66,6 +67,12 @@
   </si>
   <si>
     <t>Previous EMA (α = 0.2)</t>
+  </si>
+  <si>
+    <t>Schedule Deviation</t>
+  </si>
+  <si>
+    <t>Section</t>
   </si>
 </sst>
 </file>
@@ -127,6 +134,19 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -134,6 +154,9 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -169,22 +192,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -249,7 +256,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -489,11 +495,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1968494320"/>
-        <c:axId val="-1968498128"/>
+        <c:axId val="415135312"/>
+        <c:axId val="415135856"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1968494320"/>
+        <c:axId val="415135312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -550,12 +556,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1968498128"/>
+        <c:crossAx val="415135856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1968498128"/>
+        <c:axId val="415135856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -612,7 +618,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1968494320"/>
+        <c:crossAx val="415135312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -626,7 +632,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -733,7 +738,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -976,11 +980,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-28528672"/>
-        <c:axId val="-1968499760"/>
+        <c:axId val="416944112"/>
+        <c:axId val="416940848"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-28528672"/>
+        <c:axId val="416944112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1037,12 +1041,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1968499760"/>
+        <c:crossAx val="416940848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1968499760"/>
+        <c:axId val="416940848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1099,7 +1103,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-28528672"/>
+        <c:crossAx val="416944112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1113,7 +1117,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1220,7 +1223,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1460,11 +1462,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1852080112"/>
-        <c:axId val="-1852081744"/>
+        <c:axId val="416944656"/>
+        <c:axId val="416942480"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1852080112"/>
+        <c:axId val="416944656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1521,12 +1523,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1852081744"/>
+        <c:crossAx val="416942480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1852081744"/>
+        <c:axId val="416942480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1583,7 +1585,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1852080112"/>
+        <c:crossAx val="416944656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1597,7 +1599,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1679,7 +1680,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1940,11 +1940,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-9770016"/>
-        <c:axId val="-28517248"/>
+        <c:axId val="416943568"/>
+        <c:axId val="416945200"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-9770016"/>
+        <c:axId val="416943568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2001,12 +2001,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-28517248"/>
+        <c:crossAx val="416945200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-28517248"/>
+        <c:axId val="416945200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2063,7 +2063,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-9770016"/>
+        <c:crossAx val="416943568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2508,11 +2508,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-9774912"/>
-        <c:axId val="-9774368"/>
+        <c:axId val="416947376"/>
+        <c:axId val="417709808"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-9774912"/>
+        <c:axId val="416947376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2569,12 +2569,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-9774368"/>
+        <c:crossAx val="417709808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-9774368"/>
+        <c:axId val="417709808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2631,7 +2631,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-9774912"/>
+        <c:crossAx val="416947376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2709,6 +2709,453 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Average Schedule Deviation Along a Route</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:marker>
+              <c:symbol val="none"/>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:marker>
+              <c:symbol val="none"/>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Peak Detection Example'!$A$2:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Peak Detection Example'!$B$2:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="214455872"/>
+        <c:axId val="214462400"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="214455872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="214462400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="214462400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="214455872"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -2912,6 +3359,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -4977,6 +5464,522 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5662,23 +6665,95 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.8</cdr:x>
+      <cdr:y>0.5434</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>1</cdr:x>
+      <cdr:y>0.87674</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="TextBox 2"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="4476750" y="1490663"/>
+          <a:ext cx="914400" cy="914400"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C11" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C11" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
   <tableColumns count="3">
-    <tableColumn id="1" name="Time period" dataDxfId="6"/>
-    <tableColumn id="2" name="Observation Value" dataDxfId="5"/>
-    <tableColumn id="3" name="SMA(n=3)" dataDxfId="4"/>
+    <tableColumn id="1" name="Time period" dataDxfId="21"/>
+    <tableColumn id="2" name="Observation Value" dataDxfId="20"/>
+    <tableColumn id="3" name="SMA(n=3)" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C11" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C11" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
   <tableColumns count="3">
-    <tableColumn id="1" name="Time period" dataDxfId="11"/>
-    <tableColumn id="2" name="Observation Value" dataDxfId="10"/>
-    <tableColumn id="3" name="CMA(n=3)" dataDxfId="9"/>
+    <tableColumn id="1" name="Time period" dataDxfId="16"/>
+    <tableColumn id="2" name="Observation Value" dataDxfId="15"/>
+    <tableColumn id="3" name="CMA(n=3)" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5687,10 +6762,10 @@
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:D11" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <tableColumns count="4">
-    <tableColumn id="1" name="Time period" dataDxfId="17"/>
-    <tableColumn id="2" name="Observation Value" dataDxfId="16"/>
-    <tableColumn id="3" name="Weight moving total (n=3)" dataDxfId="15"/>
-    <tableColumn id="4" name="WMA (n=3)" dataDxfId="14">
+    <tableColumn id="1" name="Time period" dataDxfId="11"/>
+    <tableColumn id="2" name="Observation Value" dataDxfId="10"/>
+    <tableColumn id="3" name="Weight moving total (n=3)" dataDxfId="9"/>
+    <tableColumn id="4" name="WMA (n=3)" dataDxfId="8">
       <calculatedColumnFormula>C2/6</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5699,14 +6774,14 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:F11" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:F11" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <tableColumns count="6">
-    <tableColumn id="1" name="Time period" dataDxfId="23"/>
-    <tableColumn id="2" name="Observation Value" dataDxfId="22"/>
-    <tableColumn id="3" name="Previous EMA (α = 0.2)" dataDxfId="21">
+    <tableColumn id="1" name="Time period" dataDxfId="5"/>
+    <tableColumn id="2" name="Observation Value" dataDxfId="4"/>
+    <tableColumn id="3" name="Previous EMA (α = 0.2)" dataDxfId="3">
       <calculatedColumnFormula>D1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="EMA(α = 0.2)" dataDxfId="20"/>
+    <tableColumn id="4" name="EMA(α = 0.2)" dataDxfId="2"/>
     <tableColumn id="5" name="Previous EMA(α = 0.8)" dataDxfId="1"/>
     <tableColumn id="6" name="EMA(α = 0.8)" dataDxfId="0">
       <calculatedColumnFormula>Table4[[#This Row],[Observation Value]]</calculatedColumnFormula>
@@ -6421,18 +7496,18 @@
         <v>2</v>
       </c>
       <c r="J6">
-        <f t="shared" ref="J6:J16" si="1">POWER(2,I6)</f>
+        <f t="shared" ref="J6:J14" si="1">POWER(2,I6)</f>
         <v>4</v>
       </c>
       <c r="K6">
-        <f t="shared" ref="K6:K16" si="2">J6/$L$9</f>
+        <f t="shared" ref="K6:K14" si="2">J6/$L$9</f>
         <v>1.9550342130987292E-3</v>
       </c>
       <c r="N6">
         <v>2</v>
       </c>
       <c r="O6">
-        <f t="shared" ref="O6:O20" si="3">POWER(N6,2)</f>
+        <f t="shared" ref="O6:O14" si="3">POWER(N6,2)</f>
         <v>4</v>
       </c>
       <c r="P6">
@@ -6519,7 +7594,7 @@
         <v>16</v>
       </c>
       <c r="P8">
-        <f t="shared" ref="P8:P20" si="4">O8/$Q$8</f>
+        <f t="shared" ref="P8:P14" si="4">O8/$Q$8</f>
         <v>4.1558441558441558E-2</v>
       </c>
       <c r="Q8">
@@ -6743,7 +7818,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:F11"/>
     </sheetView>
   </sheetViews>
@@ -6819,7 +7894,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="3">
-        <f>$I$1*B3 + (1-$I$1)*C3</f>
+        <f t="shared" ref="D3:D10" si="0">$I$1*B3 + (1-$I$1)*C3</f>
         <v>10.4</v>
       </c>
       <c r="E3" s="2">
@@ -6839,15 +7914,15 @@
         <v>16</v>
       </c>
       <c r="C4" s="2">
-        <f t="shared" ref="C4:C11" si="0">D3</f>
+        <f t="shared" ref="C4:C11" si="1">D3</f>
         <v>10.4</v>
       </c>
       <c r="D4" s="3">
-        <f>$I$1*B4 + (1-$I$1)*C4</f>
+        <f t="shared" si="0"/>
         <v>11.52</v>
       </c>
       <c r="E4" s="2">
-        <f t="shared" ref="E4:E11" si="1">F3</f>
+        <f t="shared" ref="E4:E11" si="2">F3</f>
         <v>11.600000000000001</v>
       </c>
       <c r="F4" s="4">
@@ -6863,15 +7938,15 @@
         <v>13</v>
       </c>
       <c r="C5" s="2">
+        <f t="shared" si="1"/>
+        <v>11.52</v>
+      </c>
+      <c r="D5" s="3">
         <f t="shared" si="0"/>
-        <v>11.52</v>
-      </c>
-      <c r="D5" s="3">
-        <f>$I$1*B5 + (1-$I$1)*C5</f>
         <v>11.815999999999999</v>
       </c>
       <c r="E5" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>15.120000000000001</v>
       </c>
       <c r="F5" s="4">
@@ -6887,15 +7962,15 @@
         <v>17</v>
       </c>
       <c r="C6" s="2">
+        <f t="shared" si="1"/>
+        <v>11.815999999999999</v>
+      </c>
+      <c r="D6" s="3">
         <f t="shared" si="0"/>
-        <v>11.815999999999999</v>
-      </c>
-      <c r="D6" s="3">
-        <f>$I$1*B6 + (1-$I$1)*C6</f>
         <v>12.8528</v>
       </c>
       <c r="E6" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13.423999999999999</v>
       </c>
       <c r="F6" s="4">
@@ -6911,15 +7986,15 @@
         <v>19</v>
       </c>
       <c r="C7" s="2">
+        <f t="shared" si="1"/>
+        <v>12.8528</v>
+      </c>
+      <c r="D7" s="3">
         <f t="shared" si="0"/>
-        <v>12.8528</v>
-      </c>
-      <c r="D7" s="3">
-        <f>$I$1*B7 + (1-$I$1)*C7</f>
         <v>14.082240000000002</v>
       </c>
       <c r="E7" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>16.284800000000001</v>
       </c>
       <c r="F7" s="4">
@@ -6935,15 +8010,15 @@
         <v>15</v>
       </c>
       <c r="C8" s="2">
+        <f t="shared" si="1"/>
+        <v>14.082240000000002</v>
+      </c>
+      <c r="D8" s="3">
         <f t="shared" si="0"/>
-        <v>14.082240000000002</v>
-      </c>
-      <c r="D8" s="3">
-        <f>$I$1*B8 + (1-$I$1)*C8</f>
         <v>14.265792000000003</v>
       </c>
       <c r="E8" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>18.456960000000002</v>
       </c>
       <c r="F8" s="4">
@@ -6959,15 +8034,15 @@
         <v>20</v>
       </c>
       <c r="C9" s="2">
+        <f t="shared" si="1"/>
+        <v>14.265792000000003</v>
+      </c>
+      <c r="D9" s="3">
         <f t="shared" si="0"/>
-        <v>14.265792000000003</v>
-      </c>
-      <c r="D9" s="3">
-        <f>$I$1*B9 + (1-$I$1)*C9</f>
         <v>15.412633600000003</v>
       </c>
       <c r="E9" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>15.691392</v>
       </c>
       <c r="F9" s="4">
@@ -6983,15 +8058,15 @@
         <v>22</v>
       </c>
       <c r="C10" s="2">
+        <f t="shared" si="1"/>
+        <v>15.412633600000003</v>
+      </c>
+      <c r="D10" s="3">
         <f t="shared" si="0"/>
-        <v>15.412633600000003</v>
-      </c>
-      <c r="D10" s="3">
-        <f>$I$1*B10 + (1-$I$1)*C10</f>
         <v>16.730106880000001</v>
       </c>
       <c r="E10" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>19.138278400000001</v>
       </c>
       <c r="F10" s="4">
@@ -7007,14 +8082,14 @@
         <v>1</v>
       </c>
       <c r="C11" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16.730106880000001</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>1</v>
       </c>
       <c r="E11" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>21.427655680000001</v>
       </c>
       <c r="F11" s="4" t="s">
@@ -7033,4 +8108,151 @@
     <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U28" sqref="U28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>